<commit_message>
Added results for missing values
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CAF6DCA-DDD6-4C49-9AE1-EA860F14E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4C4FDF-CA7F-9649-B2ED-59DF7B2D8B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="2" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="137">
   <si>
     <t>Task</t>
   </si>
@@ -431,13 +431,46 @@
   </si>
   <si>
     <t>df.head() to ensure columns are dropped</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>Load Data</t>
+  </si>
+  <si>
+    <t>Use "File" widget to load the data</t>
+  </si>
+  <si>
+    <t>Inspect Missing Values</t>
+  </si>
+  <si>
+    <t>Connect to "Data Table" widget to view data</t>
+  </si>
+  <si>
+    <t>Impute Data</t>
+  </si>
+  <si>
+    <t>Use "Impute" widget to fill in missing values</t>
+  </si>
+  <si>
+    <t>Re-inspect data in "Data Table" widget</t>
+  </si>
+  <si>
+    <t>9 min</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Orange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,6 +530,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val=".AppleSystemUIFont"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val=".AppleSystemUIFont"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -518,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -527,6 +579,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,19 +914,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,10 +935,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -872,8 +949,9 @@
         <v>22</v>
       </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="21">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -881,8 +959,9 @@
         <v>13</v>
       </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="21">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -890,8 +969,9 @@
         <v>23</v>
       </c>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="21">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -899,8 +979,9 @@
         <v>10</v>
       </c>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="21">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -908,8 +989,9 @@
         <v>15</v>
       </c>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="21">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -917,8 +999,9 @@
         <v>10</v>
       </c>
       <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="21">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -926,8 +1009,9 @@
         <v>7</v>
       </c>
       <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="21">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -935,8 +1019,9 @@
         <v>10</v>
       </c>
       <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="21">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -944,8 +1029,9 @@
         <v>8</v>
       </c>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="21">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,8 +1039,9 @@
         <v>11</v>
       </c>
       <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="21">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -962,8 +1049,9 @@
         <v>10</v>
       </c>
       <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="21">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -971,8 +1059,9 @@
         <v>12</v>
       </c>
       <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="21">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -980,8 +1069,9 @@
         <v>13</v>
       </c>
       <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="21">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -989,8 +1079,9 @@
         <v>12</v>
       </c>
       <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="21">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -998,8 +1089,9 @@
         <v>11</v>
       </c>
       <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="21">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1007,8 +1099,9 @@
         <v>11</v>
       </c>
       <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="21">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1016,8 +1109,9 @@
         <v>8</v>
       </c>
       <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="21">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1025,9 +1119,10 @@
         <f>SUM(B2:B18)</f>
         <v>206</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="21">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1035,7 +1130,8 @@
         <f>B19/60</f>
         <v>3.4333333333333331</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1050,9 +1146,9 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1063,7 +1159,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1074,7 +1170,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1181,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -1096,7 +1192,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1117,9 +1213,9 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1130,7 +1226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1237,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
@@ -1152,7 +1248,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1163,7 +1259,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1174,7 +1270,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1195,9 +1291,9 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1208,7 +1304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1315,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>90</v>
       </c>
@@ -1230,7 +1326,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>92</v>
       </c>
@@ -1241,7 +1337,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1252,7 +1348,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1273,9 +1369,9 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1286,7 +1382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1297,7 +1393,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>95</v>
       </c>
@@ -1308,7 +1404,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1319,7 +1415,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1330,7 +1426,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1351,9 +1447,9 @@
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1364,7 +1460,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1375,7 +1471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>100</v>
       </c>
@@ -1386,7 +1482,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>102</v>
       </c>
@@ -1397,7 +1493,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>104</v>
       </c>
@@ -1408,7 +1504,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1419,7 +1515,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -1440,9 +1536,9 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1453,7 +1549,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1464,7 +1560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -1475,7 +1571,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>109</v>
       </c>
@@ -1486,7 +1582,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1497,7 +1593,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1518,9 +1614,9 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1531,7 +1627,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1542,7 +1638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>112</v>
       </c>
@@ -1553,7 +1649,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>114</v>
       </c>
@@ -1564,7 +1660,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1575,7 +1671,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1596,9 +1692,9 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1609,7 +1705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1620,7 +1716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
@@ -1631,7 +1727,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>118</v>
       </c>
@@ -1642,7 +1738,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1653,7 +1749,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1674,9 +1770,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1687,7 +1783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1698,7 +1794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -1709,7 +1805,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -1720,7 +1816,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1731,7 +1827,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1746,75 +1842,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" s="15" customFormat="1" ht="19">
+      <c r="A1" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="54">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="72">
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="234">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="54">
+      <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1824,92 +1990,167 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="B1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="2:12" s="15" customFormat="1" ht="19">
+      <c r="C1" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="G1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="L1" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" ht="18">
+      <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="90">
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="90">
+      <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="108">
+      <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="108">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="17">
+      <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="G7" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="2:12" ht="17">
+      <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1924,9 +2165,9 @@
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1937,7 +2178,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -1948,7 +2189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="6" t="s">
         <v>47</v>
       </c>
@@ -1959,7 +2200,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="6" t="s">
         <v>49</v>
       </c>
@@ -1970,7 +2211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1981,7 +2222,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="6" t="s">
         <v>53</v>
       </c>
@@ -1992,7 +2233,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -2014,9 +2255,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -2027,7 +2268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -2038,7 +2279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
@@ -2049,7 +2290,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -2060,7 +2301,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -2071,7 +2312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2092,9 +2333,9 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -2105,7 +2346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -2116,7 +2357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>61</v>
       </c>
@@ -2127,7 +2368,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
@@ -2138,7 +2379,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>66</v>
       </c>
@@ -2149,7 +2390,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2170,9 +2411,9 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -2183,7 +2424,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -2194,7 +2435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
@@ -2205,7 +2446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
@@ -2216,7 +2457,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -2227,7 +2468,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2248,9 +2489,9 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -2261,7 +2502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -2272,7 +2513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -2283,7 +2524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -2294,7 +2535,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -2315,9 +2556,9 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -2328,7 +2569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -2339,7 +2580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="4" t="s">
         <v>77</v>
       </c>
@@ -2350,7 +2591,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="4" t="s">
         <v>79</v>
       </c>
@@ -2361,7 +2602,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -2372,7 +2613,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Updated Orange Outlier Removal
added orange outlier removal Goms results
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4C4FDF-CA7F-9649-B2ED-59DF7B2D8B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB0088A-CD4A-7F40-90C8-C649E6D7FC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="2" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="142">
   <si>
     <t>Task</t>
   </si>
@@ -464,13 +464,28 @@
   </si>
   <si>
     <t>Orange</t>
+  </si>
+  <si>
+    <t>Use "Box Plot" widget to identify outliers</t>
+  </si>
+  <si>
+    <t>Filter Data</t>
+  </si>
+  <si>
+    <t>4 min</t>
+  </si>
+  <si>
+    <t>Set rules in "Select Rows" or use "Remove Outliers" widget</t>
+  </si>
+  <si>
+    <t>Inspect filtered data in "Data Table" widget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,6 +564,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -570,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,7 +599,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -598,6 +618,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1851,21 +1883,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="9" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="15" customFormat="1" ht="19">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:9" s="14" customFormat="1" ht="19">
+      <c r="A1" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1876,16 +1908,16 @@
       <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1896,16 +1928,16 @@
       <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1916,16 +1948,16 @@
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1936,16 +1968,16 @@
       <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1956,16 +1988,16 @@
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1976,10 +2008,10 @@
       <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1990,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
-  <dimension ref="B1:L8"/>
+  <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2005,20 +2037,20 @@
     <col min="8" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="15" customFormat="1" ht="19">
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="L1" s="15" t="s">
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="18">
+    <row r="2" spans="2:11" ht="18">
       <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2029,17 +2061,17 @@
         <v>38</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="90">
+    <row r="3" spans="2:11" ht="90">
       <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
@@ -2050,17 +2082,17 @@
         <v>27</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="90">
+    <row r="4" spans="2:11" ht="90">
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
@@ -2071,17 +2103,17 @@
         <v>41</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="108">
+    <row r="5" spans="2:11" ht="108">
       <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
@@ -2092,17 +2124,17 @@
         <v>43</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="108">
+    <row r="6" spans="2:11" ht="108">
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2113,17 +2145,17 @@
         <v>44</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="17">
+    <row r="7" spans="2:11" ht="17">
       <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
@@ -2134,15 +2166,15 @@
         <v>41</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="2:12" ht="17">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="2:11" ht="17">
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
@@ -2159,88 +2191,159 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D2" s="17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="6" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="90">
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D3" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="6" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="90">
+      <c r="B4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D4" s="18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="6" t="s">
+      <c r="F4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="G4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="126">
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D5" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="6" t="s">
+      <c r="F5" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="108">
+      <c r="B6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D6" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="6" t="s">
+      <c r="F6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="G6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="72">
+      <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D7" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17">
-      <c r="A7" s="5" t="s">
+      <c r="F7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="G7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="2:11" ht="17">
+      <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="D8" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added numeric to categorical results
Updated GOMS by adding the numeric to Categorical results from Orange
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB0088A-CD4A-7F40-90C8-C649E6D7FC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B372D-047C-9744-A105-ED2FE3D50293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="2" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="4" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="147">
   <si>
     <t>Task</t>
   </si>
@@ -479,6 +479,21 @@
   </si>
   <si>
     <t>Inspect filtered data in "Data Table" widget</t>
+  </si>
+  <si>
+    <t>Use "File" widget to load the dataset</t>
+  </si>
+  <si>
+    <t>Convert Types</t>
+  </si>
+  <si>
+    <t>Use "Edit Domain" widget to change attribute type</t>
+  </si>
+  <si>
+    <t>Use "Data Table" widget to verify changes</t>
+  </si>
+  <si>
+    <t>6 min</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -2194,7 +2209,7 @@
   <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2352,74 +2367,136 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE8F680-674B-C845-897A-B307A627C944}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="90">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="108">
+      <c r="B4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="108">
+      <c r="B5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="H5" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="54">
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="G6" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added PCA results into GOMS
Updated the Orange results into our GOMS Excel
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B372D-047C-9744-A105-ED2FE3D50293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6061A1-26A7-634B-A06C-0507F067F2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="4" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="5" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="151">
   <si>
     <t>Task</t>
   </si>
@@ -494,6 +494,18 @@
   </si>
   <si>
     <t>6 min</t>
+  </si>
+  <si>
+    <t>Use 'File' widget to load the dataset</t>
+  </si>
+  <si>
+    <t>Connect 'PCA' widget and set parameters</t>
+  </si>
+  <si>
+    <t>Visualize Results</t>
+  </si>
+  <si>
+    <t>Connect 'Scatter Plot' widget to visualize PCA results</t>
   </si>
 </sst>
 </file>
@@ -2369,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE8F680-674B-C845-897A-B307A627C944}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2507,74 +2519,134 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC162D1-E2CB-9148-882F-73C6122D3717}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="8" max="8" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="108">
+      <c r="B4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="G4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="126">
+      <c r="B5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="90">
+      <c r="B6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="G6" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated change column name
updated GOMS rename column feature in orange
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6061A1-26A7-634B-A06C-0507F067F2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A636A06A-53D9-D148-9256-62658B70D396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="5" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="7" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="154">
   <si>
     <t>Task</t>
   </si>
@@ -506,6 +506,15 @@
   </si>
   <si>
     <t>Connect 'Scatter Plot' widget to visualize PCA results</t>
+  </si>
+  <si>
+    <t>Edit Domain</t>
+  </si>
+  <si>
+    <t>Use 'Edit Domain' widget to rename columns</t>
+  </si>
+  <si>
+    <t>Inspect with 'Data Table' widget</t>
   </si>
 </sst>
 </file>
@@ -2521,8 +2530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC162D1-E2CB-9148-882F-73C6122D3717}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2657,74 +2666,134 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87741834-764D-8442-88E6-1252B0C99BC2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="8" max="8" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="90">
+      <c r="B4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="108">
+      <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="H5" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="54">
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="G6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2735,65 +2804,124 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="B1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="90">
+      <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="3" t="s">
+      <c r="F5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="17">
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="F6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated chnage column type GOMS
Added change column type results GOMS orange
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A636A06A-53D9-D148-9256-62658B70D396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95980A9C-3E5F-1F46-A0A0-06691F6FF270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="7" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="6" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="157">
   <si>
     <t>Task</t>
   </si>
@@ -515,6 +515,15 @@
   </si>
   <si>
     <t>Inspect with 'Data Table' widget</t>
+  </si>
+  <si>
+    <t>Use the 'File' widget to load the dataset.</t>
+  </si>
+  <si>
+    <t>Use the 'Edit Domain' widget to change the feature type.</t>
+  </si>
+  <si>
+    <t>Inspect the changes in the 'Data Table' widget.</t>
   </si>
 </sst>
 </file>
@@ -2668,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87741834-764D-8442-88E6-1252B0C99BC2}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2701,17 +2710,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" ht="90">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2728,10 +2737,10 @@
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="90">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="144">
       <c r="B4" s="4" t="s">
         <v>69</v>
       </c>
@@ -2745,13 +2754,13 @@
         <v>151</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="108">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="126">
       <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>40</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="54">
@@ -2785,7 +2794,7 @@
         <v>36</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
       <c r="H6" s="16"/>
     </row>
@@ -2806,7 +2815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
   <dimension ref="B1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Special Character Removal Results
As described GOMS updated
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95980A9C-3E5F-1F46-A0A0-06691F6FF270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EDBB7D-D369-F543-84A7-37436DDEF67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="6" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="8" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="173">
   <si>
     <t>Task</t>
   </si>
@@ -481,33 +481,9 @@
     <t>Inspect filtered data in "Data Table" widget</t>
   </si>
   <si>
-    <t>Use "File" widget to load the dataset</t>
-  </si>
-  <si>
-    <t>Convert Types</t>
-  </si>
-  <si>
-    <t>Use "Edit Domain" widget to change attribute type</t>
-  </si>
-  <si>
-    <t>Use "Data Table" widget to verify changes</t>
-  </si>
-  <si>
-    <t>6 min</t>
-  </si>
-  <si>
     <t>Use 'File' widget to load the dataset</t>
   </si>
   <si>
-    <t>Connect 'PCA' widget and set parameters</t>
-  </si>
-  <si>
-    <t>Visualize Results</t>
-  </si>
-  <si>
-    <t>Connect 'Scatter Plot' widget to visualize PCA results</t>
-  </si>
-  <si>
     <t>Edit Domain</t>
   </si>
   <si>
@@ -523,7 +499,79 @@
     <t>Use the 'Edit Domain' widget to change the feature type.</t>
   </si>
   <si>
-    <t>Inspect the changes in the 'Data Table' widget.</t>
+    <t>Preprocess</t>
+  </si>
+  <si>
+    <t>Inspect Data Types</t>
+  </si>
+  <si>
+    <t>Connect 'Data Table' widget to review current data types.</t>
+  </si>
+  <si>
+    <t>Re-inspect in 'Data Table' widget to confirm the changes.</t>
+  </si>
+  <si>
+    <t>Use 'File' widget to load the dataset.</t>
+  </si>
+  <si>
+    <t>Inspect Data Distribution</t>
+  </si>
+  <si>
+    <t>Connect 'Box Plot' or 'Distributions' widget to view data spread.</t>
+  </si>
+  <si>
+    <t>Use 'Preprocess' widget, select 'Normalize' to scale the data.</t>
+  </si>
+  <si>
+    <t>Re-inspect with 'Data Table' or 'Distributions' widget.</t>
+  </si>
+  <si>
+    <t>Inspect Numeric Columns</t>
+  </si>
+  <si>
+    <t>Connect 'Data Table' widget to identify numeric columns.</t>
+  </si>
+  <si>
+    <t>Convert Type</t>
+  </si>
+  <si>
+    <t>Use 'Edit Domain' widget to change numeric to categorical.</t>
+  </si>
+  <si>
+    <t>Verify Conversion</t>
+  </si>
+  <si>
+    <t>Re-inspect with 'Data Table' to check the new column type.</t>
+  </si>
+  <si>
+    <t>Use 'Preprocess' widget and select 'Scale'.</t>
+  </si>
+  <si>
+    <t>Connect 'PCA' widget and set parameters.</t>
+  </si>
+  <si>
+    <t>Visualize PCA</t>
+  </si>
+  <si>
+    <t>Connect 'Scatter Plot' widget to the PCA output to visualize components.</t>
+  </si>
+  <si>
+    <t>Inspect Text Data</t>
+  </si>
+  <si>
+    <t>Connect 'Data Table' widget to view text data.</t>
+  </si>
+  <si>
+    <t>Remove Special Characters</t>
+  </si>
+  <si>
+    <t>Use 'Preprocess Text' widget with 'Remove Special Characters'.</t>
+  </si>
+  <si>
+    <t>Verify Removal</t>
+  </si>
+  <si>
+    <t>Re-inspect with 'Data Table' widget to check the text.</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1042,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1919,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1930,23 +1978,23 @@
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="9" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="19">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
         <v>135</v>
       </c>
       <c r="D1" s="15"/>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>136</v>
       </c>
       <c r="H1" s="15"/>
-      <c r="I1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="2:11" ht="18">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1966,7 +2014,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="54">
+    <row r="3" spans="2:11" ht="54">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1976,17 +2024,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="72">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="72">
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1996,17 +2044,17 @@
       <c r="D4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>34</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="234">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="234">
       <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
@@ -2016,17 +2064,17 @@
       <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>62</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="54">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="72">
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
@@ -2036,29 +2084,30 @@
       <c r="D6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>34</v>
+      <c r="G6" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>134</v>
-      </c>
+      <c r="G7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2069,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -2238,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="F3:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2399,16 +2448,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE8F680-674B-C845-897A-B307A627C944}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
@@ -2444,7 +2493,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="90">
+    <row r="3" spans="2:11" ht="72">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2454,17 +2503,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="108">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126">
       <c r="B4" s="4" t="s">
         <v>56</v>
       </c>
@@ -2474,17 +2523,17 @@
       <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>62</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="108">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="144">
       <c r="B5" s="4" t="s">
         <v>58</v>
       </c>
@@ -2494,17 +2543,17 @@
       <c r="D5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>40</v>
+      <c r="F5" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="54">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="162">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2514,21 +2563,30 @@
       <c r="D6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="2:11" ht="17">
+      <c r="F6" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2539,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC162D1-E2CB-9148-882F-73C6122D3717}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2592,17 +2650,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="108">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126">
       <c r="B4" s="4" t="s">
         <v>61</v>
       </c>
@@ -2612,17 +2670,17 @@
       <c r="D4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>62</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="126">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="108">
       <c r="B5" s="4" t="s">
         <v>64</v>
       </c>
@@ -2632,17 +2690,17 @@
       <c r="D5" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>34</v>
+      <c r="F5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="90">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="180">
       <c r="B6" s="4" t="s">
         <v>66</v>
       </c>
@@ -2652,21 +2710,30 @@
       <c r="D6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="2:11" ht="17">
+      <c r="F6" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2677,8 +2744,281 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87741834-764D-8442-88E6-1252B0C99BC2}">
   <dimension ref="B1:K7"/>
   <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="90">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="144">
+      <c r="B4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="144">
+      <c r="B5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="90">
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
+  <dimension ref="B1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126">
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="90">
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="17">
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
+  <dimension ref="B1:K7"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2720,7 +3060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="90">
+    <row r="3" spans="2:11" ht="72">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2737,50 +3077,50 @@
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="144">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="108">
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>62</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="126">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="162">
       <c r="B5" s="4" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="54">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="144">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2788,15 +3128,17 @@
         <v>40</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H6" s="16"/>
+        <v>81</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="17">
       <c r="B7" s="3" t="s">
@@ -2805,210 +3147,13 @@
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
-  <dimension ref="B1:K6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" ht="18">
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="72">
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="126">
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="90">
-      <c r="B5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="17">
-      <c r="B6" s="3" t="s">
+      <c r="F7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="G7" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Trim Whitespaces results
Updated GOMS trim white spaces results Orange
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EDBB7D-D369-F543-84A7-37436DDEF67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35AA70D-83E4-9E43-8B7D-5F73858B9389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="8" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="5" activeTab="9" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="177">
   <si>
     <t>Task</t>
   </si>
@@ -572,6 +572,18 @@
   </si>
   <si>
     <t>Re-inspect with 'Data Table' widget to check the text.</t>
+  </si>
+  <si>
+    <t>Inspect Whitespace</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' to view whitespace issues.</t>
+  </si>
+  <si>
+    <t>Connect 'Preprocess Text', add 'Strip Whitespace'.</t>
+  </si>
+  <si>
+    <t>Re-inspect with 'Data Table'.</t>
   </si>
 </sst>
 </file>
@@ -1265,65 +1277,137 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6062ED13-C528-F146-AE70-5ACC98E5FD07}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="144">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="144">
+      <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="3" t="s">
+      <c r="F5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="90">
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="F6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3017,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added Text Case Results
Results added GOMS
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B295BF-89D5-AD4B-A160-E139F8CF49E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E951139F-1576-2042-A510-545111FF5F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="6" activeTab="10" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="6" activeTab="11" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="184">
   <si>
     <t>Task</t>
   </si>
@@ -593,6 +593,18 @@
   </si>
   <si>
     <t>Use 'Preprocess Text' to configure replacements.</t>
+  </si>
+  <si>
+    <t>Inspect Text Case</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' to view text case.</t>
+  </si>
+  <si>
+    <t>Change Text Case</t>
+  </si>
+  <si>
+    <t>Connect 'Preprocess Text', select 'Change Case'.</t>
   </si>
 </sst>
 </file>
@@ -1427,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20D2886-70F8-A640-969D-1FFF78906280}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1573,76 +1585,146 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B17B441-DAD5-B14A-B665-039BC5DFC85A}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126">
+      <c r="B4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="126">
+      <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="108">
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Collapse Rare Category results
added results GOMS
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257D13EE-63B0-7449-B510-019F1F247588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0ADB3A-2F56-DB45-88A3-A3BD062DC67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="13" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="189">
   <si>
     <t>Task</t>
   </si>
@@ -611,6 +611,15 @@
   </si>
   <si>
     <t>Connect 'Preprocess Text', add 'Remove Stopwords'.</t>
+  </si>
+  <si>
+    <t>Visualize Categories</t>
+  </si>
+  <si>
+    <t>Use 'Bar Chart' to view category frequencies.</t>
+  </si>
+  <si>
+    <t>Use 'Edit Domain' or 'Python Script' to collapse rare categories.</t>
   </si>
 </sst>
 </file>
@@ -1742,7 +1751,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1887,85 +1896,156 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990E6A3-2F89-4543-9085-4F79AE6CF6C1}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="108">
+      <c r="B4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="162">
+      <c r="B5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="H5" s="13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="198">
+      <c r="B6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="4" t="s">
+      <c r="F6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="G6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="H6" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="72">
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17">
-      <c r="A7" s="3" t="s">
+      <c r="F7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="G7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="2:11" ht="17">
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Datetime Components Results
results GOMS
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD179275-89FE-4344-84F5-8AA0C08E6495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1779B3D-CB1D-DE46-835E-96B8112E7F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="10" activeTab="15" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="12" activeTab="16" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="195">
   <si>
     <t>Task</t>
   </si>
@@ -629,6 +629,15 @@
   </si>
   <si>
     <t>Connect 'Preprocess Text', configure 'Regex'.</t>
+  </si>
+  <si>
+    <t>Inspect Datetime Data</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' to review datetime columns.</t>
+  </si>
+  <si>
+    <t>Use 'Date' widget to extract date components.</t>
   </si>
 </sst>
 </file>
@@ -2216,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDFEC69-75A2-0441-AC67-AB453D872A52}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2363,76 +2372,147 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779DF32-F3C5-8D4E-BC6D-C6BF3912FD45}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126">
+      <c r="B4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="126">
+      <c r="B5" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="90">
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added remove Columns Results
Results GOMS
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1779B3D-CB1D-DE46-835E-96B8112E7F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1556FAE-6D73-E14A-BE90-62AFC39DEBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="12" activeTab="16" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="13" activeTab="17" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="198">
   <si>
     <t>Task</t>
   </si>
@@ -638,6 +638,15 @@
   </si>
   <si>
     <t>Use 'Date' widget to extract date components.</t>
+  </si>
+  <si>
+    <t>Inspect Columns</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' to decide which columns to remove.</t>
+  </si>
+  <si>
+    <t>Use 'Select Columns' to deselect unwanted columns.</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779DF32-F3C5-8D4E-BC6D-C6BF3912FD45}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -2521,76 +2530,147 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836C7B9-0B85-3A4B-822E-23EEAE7381E3}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="18">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="4" t="s">
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="72">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="144">
+      <c r="B4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="144">
+      <c r="B5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="4" t="s">
+      <c r="F5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="90">
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Layout for better visibility
Updated Goms Layout :smile
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1556FAE-6D73-E14A-BE90-62AFC39DEBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE61DF2-E11F-074A-B914-08A5ED14800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="13" activeTab="17" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="13" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -714,29 +714,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val=".AppleSystemUIFont"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val=".AppleSystemUIFont"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -759,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -773,22 +756,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -798,6 +767,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1117,17 +1090,17 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A18"/>
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21">
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1151,7 +1124,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="21">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1134,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="21">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1171,7 +1144,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="21">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1154,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="21">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1164,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="21">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1201,7 +1174,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="21">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1211,7 +1184,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="21">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1221,7 +1194,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="21">
+    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1231,7 +1204,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="21">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1241,7 +1214,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="21">
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1224,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="21">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1261,7 +1234,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="21">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1271,7 +1244,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="21">
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1281,7 +1254,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="21">
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1291,7 +1264,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="21">
+    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1301,7 +1274,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="21">
+    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1311,7 +1284,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="21">
+    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1322,7 +1295,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="21">
+    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1343,30 +1316,34 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="15" style="14" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1376,17 +1353,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1396,17 +1373,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="144">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1416,17 +1393,17 @@
       <c r="D4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="144">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1436,41 +1413,43 @@
       <c r="D5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="D6" s="15"/>
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
-      <c r="F7" s="10" t="s">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1482,30 +1461,34 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="21" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1515,17 +1498,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1535,17 +1518,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>85</v>
       </c>
@@ -1555,17 +1538,17 @@
       <c r="D4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="144">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1575,17 +1558,17 @@
       <c r="D5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1595,30 +1578,31 @@
       <c r="D6" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1630,30 +1614,34 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="20" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1663,17 +1651,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1683,17 +1671,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>90</v>
       </c>
@@ -1703,17 +1691,17 @@
       <c r="D4" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="126">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
@@ -1723,17 +1711,17 @@
       <c r="D5" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="108">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1743,30 +1731,31 @@
       <c r="D6" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1778,30 +1767,34 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="9" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="21.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="14.83203125" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1811,17 +1804,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1831,17 +1824,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="90">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>95</v>
       </c>
@@ -1851,17 +1844,17 @@
       <c r="D4" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="144">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1871,17 +1864,17 @@
       <c r="D5" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1891,30 +1884,31 @@
       <c r="D6" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1925,32 +1919,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990E6A3-2F89-4543-9085-4F79AE6CF6C1}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="18.83203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="17.5" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1960,17 +1959,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1980,17 +1979,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="108">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>100</v>
       </c>
@@ -2000,17 +1999,17 @@
       <c r="D4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="162">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>102</v>
       </c>
@@ -2020,17 +2019,17 @@
       <c r="D5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="198">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>104</v>
       </c>
@@ -2040,17 +2039,17 @@
       <c r="D6" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="72">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
@@ -2060,21 +2059,23 @@
       <c r="D7" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="2:11" ht="17">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="D8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2086,31 +2087,36 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="14.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="20.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="20.1640625" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2120,17 +2126,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2140,17 +2146,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="90">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>107</v>
       </c>
@@ -2160,17 +2166,17 @@
       <c r="D4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="126">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>109</v>
       </c>
@@ -2180,17 +2186,17 @@
       <c r="D5" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2200,30 +2206,31 @@
       <c r="D6" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2235,31 +2242,36 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="9" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="20" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="20" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2269,17 +2281,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2289,17 +2301,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>112</v>
       </c>
@@ -2309,17 +2321,17 @@
       <c r="D4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="126">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>114</v>
       </c>
@@ -2329,17 +2341,17 @@
       <c r="D5" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2349,30 +2361,31 @@
       <c r="D6" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2384,31 +2397,36 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="24.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="24" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="24.1640625" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2418,17 +2436,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2438,17 +2456,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>116</v>
       </c>
@@ -2458,17 +2476,17 @@
       <c r="D4" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="126">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>118</v>
       </c>
@@ -2478,17 +2496,17 @@
       <c r="D5" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2498,30 +2516,31 @@
       <c r="D6" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2532,32 +2551,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836C7B9-0B85-3A4B-822E-23EEAE7381E3}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="24.5" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="24.5" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2567,17 +2591,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2587,17 +2611,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="144">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>121</v>
       </c>
@@ -2607,17 +2631,17 @@
       <c r="D4" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="144">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>123</v>
       </c>
@@ -2627,17 +2651,17 @@
       <c r="D5" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2647,30 +2671,31 @@
       <c r="D6" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2682,31 +2707,36 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+      <selection activeCell="H10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="15.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="22.6640625" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2716,17 +2746,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="54">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -2736,17 +2766,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="72">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
@@ -2756,17 +2786,17 @@
       <c r="D4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="234">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="234" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
@@ -2776,17 +2806,17 @@
       <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="72">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
@@ -2796,30 +2826,31 @@
       <c r="D6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2831,32 +2862,36 @@
   <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="D9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="41.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="21.5" style="14" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2867,17 +2902,17 @@
         <v>38</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="90">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
@@ -2888,17 +2923,17 @@
         <v>27</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="90">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
@@ -2909,17 +2944,17 @@
         <v>41</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="108">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
@@ -2930,17 +2965,17 @@
         <v>43</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="108">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2951,17 +2986,17 @@
         <v>44</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
@@ -2972,15 +3007,15 @@
         <v>41</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="2:11" ht="17">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
@@ -2999,157 +3034,163 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="F3:H8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="90">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="90">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="126">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="108">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="72">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="2:11" ht="17">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="13"/>
+      <c r="H8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3160,32 +3201,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE8F680-674B-C845-897A-B307A627C944}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="13.1640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="16.33203125" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3195,17 +3241,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -3215,17 +3261,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>56</v>
       </c>
@@ -3235,17 +3281,17 @@
       <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="144">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>58</v>
       </c>
@@ -3255,17 +3301,17 @@
       <c r="D5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="162">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3275,30 +3321,31 @@
       <c r="D6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3310,29 +3357,32 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G7" sqref="F7:G7"/>
+      <selection activeCell="K12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3342,17 +3392,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -3362,17 +3412,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>61</v>
       </c>
@@ -3382,17 +3432,17 @@
       <c r="D4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="108">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>64</v>
       </c>
@@ -3402,17 +3452,17 @@
       <c r="D5" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="180">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="162" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>66</v>
       </c>
@@ -3422,30 +3472,31 @@
       <c r="D6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3457,30 +3508,34 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+      <selection activeCell="J6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="9" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="14" style="14" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="16.5" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3490,17 +3545,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="90">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -3510,17 +3565,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="144">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>69</v>
       </c>
@@ -3530,17 +3585,17 @@
       <c r="D4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="144">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
@@ -3550,17 +3605,17 @@
       <c r="D5" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="90">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3570,29 +3625,31 @@
       <c r="D6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3604,28 +3661,30 @@
   <dimension ref="B1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3635,17 +3694,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -3655,17 +3714,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="126">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
@@ -3675,17 +3734,17 @@
       <c r="D4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="90">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
@@ -3695,30 +3754,31 @@
       <c r="D5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="17">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="D6" s="15"/>
+      <c r="F6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="16"/>
+      <c r="H6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3729,30 +3789,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="5" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="19">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="10"/>
+      <c r="G1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18">
+    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3762,17 +3825,17 @@
       <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="72">
+    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -3782,17 +3845,17 @@
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="108">
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>77</v>
       </c>
@@ -3802,17 +3865,17 @@
       <c r="D4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="162">
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="162" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>79</v>
       </c>
@@ -3822,17 +3885,17 @@
       <c r="D5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="144">
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3842,30 +3905,31 @@
       <c r="D6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17">
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the comparison Page
Results .sum per min and hour added
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE61DF2-E11F-074A-B914-08A5ED14800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0D70F3-E6AC-AB49-A6F0-FA9E9646F467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="13" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="198">
   <si>
     <t>Task</t>
   </si>
@@ -1089,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,7 +1121,9 @@
       <c r="B2" s="2">
         <v>22</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>8</v>
+      </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1131,7 +1133,9 @@
       <c r="B3" s="2">
         <v>13</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>9</v>
+      </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1141,7 +1145,9 @@
       <c r="B4" s="2">
         <v>23</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>13</v>
+      </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1151,7 +1157,9 @@
       <c r="B5" s="2">
         <v>10</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>10</v>
+      </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1161,7 +1169,9 @@
       <c r="B6" s="2">
         <v>15</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2">
+        <v>11</v>
+      </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1171,7 +1181,9 @@
       <c r="B7" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1181,7 +1193,9 @@
       <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1191,7 +1205,9 @@
       <c r="B9" s="2">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1201,7 +1217,9 @@
       <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1211,7 +1229,9 @@
       <c r="B11" s="2">
         <v>11</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>9</v>
+      </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1221,7 +1241,9 @@
       <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <v>7</v>
+      </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1231,7 +1253,9 @@
       <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1241,7 +1265,9 @@
       <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1251,7 +1277,9 @@
       <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1259,9 +1287,11 @@
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8</v>
+      </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1269,9 +1299,11 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C17" s="2">
+        <v>7</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1279,9 +1311,11 @@
         <v>19</v>
       </c>
       <c r="B18" s="2">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7</v>
+      </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1290,9 +1324,12 @@
       </c>
       <c r="B19" s="1">
         <f>SUM(B2:B18)</f>
-        <v>206</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>195</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUM(C2:C18)</f>
+        <v>146</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1301,9 +1338,12 @@
       </c>
       <c r="B20" s="1">
         <f>B19/60</f>
-        <v>3.4333333333333331</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="C20" s="1">
+        <f>C19/60</f>
+        <v>2.4333333333333331</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
   </sheetData>
@@ -1316,7 +1356,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="A1:XFD1048576"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1461,7 +1501,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="A1:XFD1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1508,7 +1548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1528,7 +1568,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>85</v>
       </c>
@@ -1542,13 +1582,13 @@
         <v>177</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="144" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +1608,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1588,21 +1628,19 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1613,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B17B441-DAD5-B14A-B665-039BC5DFC85A}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1641,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1661,7 +1699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1681,7 +1719,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>90</v>
       </c>
@@ -1695,13 +1733,13 @@
         <v>180</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
@@ -1721,7 +1759,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1741,21 +1779,19 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1917,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990E6A3-2F89-4543-9085-4F79AE6CF6C1}">
-  <dimension ref="B1:K8"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1949,7 +1985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1969,7 +2005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1989,7 +2025,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>100</v>
       </c>
@@ -2009,7 +2045,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>102</v>
       </c>
@@ -2020,16 +2056,16 @@
         <v>103</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>104</v>
       </c>
@@ -2040,16 +2076,16 @@
         <v>105</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
@@ -2059,23 +2095,43 @@
       <c r="D7" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2087,7 +2143,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="A1:XFD1048576"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2242,7 +2298,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="A1:XFD1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2271,7 +2327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2291,12 +2347,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>27</v>
@@ -2311,7 +2367,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>112</v>
       </c>
@@ -2331,7 +2387,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>114</v>
       </c>
@@ -2351,7 +2407,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2371,21 +2427,19 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>84</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2397,7 +2451,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="A1:XFD1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2426,7 +2480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2446,12 +2500,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>27</v>
@@ -2460,13 +2514,13 @@
         <v>127</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>116</v>
       </c>
@@ -2486,7 +2540,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>118</v>
       </c>
@@ -2506,7 +2560,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2526,21 +2580,19 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>76</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2551,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836C7B9-0B85-3A4B-822E-23EEAE7381E3}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K6" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2581,7 +2633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2601,12 +2653,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>27</v>
@@ -2615,13 +2667,13 @@
         <v>127</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>121</v>
       </c>
@@ -2641,7 +2693,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>123</v>
       </c>
@@ -2661,7 +2713,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2681,21 +2733,19 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>139</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
renamed columns due to confusion and poor naming
updated minor change to column names
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0D70F3-E6AC-AB49-A6F0-FA9E9646F467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96366779-3DA2-654C-B3E1-D6187BB67F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Local IDE ( PYTHON ) in minutes</t>
-  </si>
-  <si>
     <t>Data Polish</t>
   </si>
   <si>
@@ -433,9 +430,6 @@
     <t>df.head() to ensure columns are dropped</t>
   </si>
   <si>
-    <t>ORANGE</t>
-  </si>
-  <si>
     <t>Load Data</t>
   </si>
   <si>
@@ -647,6 +641,12 @@
   </si>
   <si>
     <t>Use 'Select Columns' to deselect unwanted columns.</t>
+  </si>
+  <si>
+    <t>Python (min)</t>
+  </si>
+  <si>
+    <t>ORANGE (min)</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,18 +1105,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>22</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>13</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>23</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>15</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>8</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>11</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>12</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>8</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>7</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
         <v>4</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
         <f>SUM(B2:B18)</f>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <f>B19/60</f>
@@ -1372,122 +1372,122 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="15"/>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -1517,129 +1517,129 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="144" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1668,129 +1668,129 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1819,130 +1819,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>96</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -1974,149 +1974,149 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="F5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -2161,130 +2161,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -2316,129 +2316,129 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2469,129 +2469,129 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>119</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2622,129 +2622,129 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>124</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2775,130 +2775,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="234" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -2930,147 +2930,147 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -3103,141 +3103,141 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="F4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>50</v>
-      </c>
       <c r="F5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>54</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="13"/>
       <c r="H8" s="15"/>
@@ -3270,130 +3270,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -3421,130 +3421,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="F4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="H4" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="162" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -3574,130 +3574,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -3723,110 +3723,110 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="15"/>
       <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="15"/>
     </row>
@@ -3854,130 +3854,130 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="14" customFormat="1" ht="162" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="15"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="15"/>
     </row>

</xml_diff>

<commit_message>
Half way though updating (lunch break)
updating sheet to make sure all is up to date, still working progress
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96366779-3DA2-654C-B3E1-D6187BB67F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94195783-EE27-4C49-AD79-427B04530741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" activeTab="5" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="193">
   <si>
     <t>Task</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Overall</t>
   </si>
   <si>
-    <t>22 min</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>Verify</t>
   </si>
   <si>
-    <t>13 min</t>
-  </si>
-  <si>
     <t>Statistical Summary</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>Replot with sns.boxplot(data=df)</t>
   </si>
   <si>
-    <t>23 min</t>
-  </si>
-  <si>
     <t>Identify Numerics</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>explained_variance_ratio_ to check variance</t>
   </si>
   <si>
-    <t>15 min</t>
-  </si>
-  <si>
     <t>Identify Column &amp; Type</t>
   </si>
   <si>
@@ -319,9 +307,6 @@
     <t>df['column'].unique() to check replacements</t>
   </si>
   <si>
-    <t>11 min</t>
-  </si>
-  <si>
     <t>Identify Text Columns</t>
   </si>
   <si>
@@ -349,9 +334,6 @@
     <t>Print some text samples to check</t>
   </si>
   <si>
-    <t>12 min</t>
-  </si>
-  <si>
     <t>Value Counts</t>
   </si>
   <si>
@@ -473,6 +455,9 @@
   </si>
   <si>
     <t>Inspect filtered data in "Data Table" widget</t>
+  </si>
+  <si>
+    <t>6 min</t>
   </si>
   <si>
     <t>Use 'File' widget to load the dataset</t>
@@ -1089,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1119,9 +1104,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>22</v>
+        <f>Normalisation!C7</f>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
+        <f>Normalisation!G7</f>
         <v>8</v>
       </c>
       <c r="D2" s="2"/>
@@ -1131,9 +1118,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>13</v>
+        <f>'Missing Values'!C8</f>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
+        <f>'Missing Values'!G7</f>
         <v>9</v>
       </c>
       <c r="D3" s="2"/>
@@ -1143,9 +1132,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>23</v>
+        <f>'Outlier Removal'!C8</f>
+        <v>19</v>
       </c>
       <c r="C4" s="2">
+        <f>'Outlier Removal'!G7</f>
         <v>13</v>
       </c>
       <c r="D4" s="2"/>
@@ -1155,9 +1146,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>10</v>
+        <f>'Numeric To Categorical'!C7</f>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
+        <f>'Numeric To Categorical'!G7</f>
         <v>10</v>
       </c>
       <c r="D5" s="2"/>
@@ -1167,10 +1160,12 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>15</v>
+        <f>'Missing Values'!C11</f>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>11</v>
+        <f>'Missing Values'!G10</f>
+        <v>0</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -1179,10 +1174,12 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <f>'Outlier Removal'!C11</f>
+        <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
+        <f>'Outlier Removal'!G10</f>
+        <v>0</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -1191,10 +1188,12 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>7</v>
+        <f>Normalisation!C13</f>
+        <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
+        <f>Normalisation!G13</f>
+        <v>0</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -1203,10 +1202,12 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>10</v>
+        <f>'Missing Values'!C14</f>
+        <v>0</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <f>'Missing Values'!G13</f>
+        <v>0</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1215,10 +1216,12 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>8</v>
+        <f>'Outlier Removal'!C14</f>
+        <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>8</v>
+        <f>'Outlier Removal'!G13</f>
+        <v>0</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -1227,10 +1230,12 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>11</v>
+        <f>Normalisation!C16</f>
+        <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>9</v>
+        <f>Normalisation!G16</f>
+        <v>0</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1239,10 +1244,12 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>10</v>
+        <f>'Missing Values'!C17</f>
+        <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>7</v>
+        <f>'Missing Values'!G16</f>
+        <v>0</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1251,10 +1258,12 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>12</v>
+        <f>'Outlier Removal'!C17</f>
+        <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>8</v>
+        <f>'Outlier Removal'!G16</f>
+        <v>0</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -1263,10 +1272,12 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>13</v>
+        <f>Normalisation!C19</f>
+        <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>10</v>
+        <f>Normalisation!G19</f>
+        <v>0</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -1275,10 +1286,12 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>12</v>
+        <f>'Missing Values'!C20</f>
+        <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>8</v>
+        <f>'Missing Values'!G19</f>
+        <v>0</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -1287,10 +1300,12 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>8</v>
+        <f>'Outlier Removal'!C20</f>
+        <v>0</v>
       </c>
       <c r="C16" s="2">
-        <v>8</v>
+        <f>'Outlier Removal'!G19</f>
+        <v>0</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1299,10 +1314,12 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>7</v>
+        <f>Normalisation!C22</f>
+        <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>7</v>
+        <f>Normalisation!G22</f>
+        <v>0</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -1311,10 +1328,12 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <f>'Missing Values'!C23</f>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>7</v>
+        <f>'Missing Values'!G22</f>
+        <v>0</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -1324,11 +1343,11 @@
       </c>
       <c r="B19" s="1">
         <f>SUM(B2:B18)</f>
-        <v>195</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>146</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -1338,11 +1357,11 @@
       </c>
       <c r="B20" s="1">
         <f>B19/60</f>
-        <v>3.25</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="C20" s="1">
         <f>C19/60</f>
-        <v>2.4333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1355,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6062ED13-C528-F146-AE70-5ACC98E5FD07}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,18 +1391,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1403,27 +1422,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="144" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1431,65 +1450,62 @@
         <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>25</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="D7" s="15"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1500,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20D2886-70F8-A640-969D-1FFF78906280}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,11 +1533,11 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -1553,39 +1569,39 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="144" x14ac:dyDescent="0.2">
@@ -1596,36 +1612,36 @@
         <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -1633,13 +1649,13 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1652,7 +1668,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,11 +1684,11 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -1704,79 +1720,79 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -1784,13 +1800,13 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1803,7 +1819,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="A1:XFD1048576"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1819,18 +1835,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1850,47 +1866,47 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1898,53 +1914,51 @@
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>79</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1956,7 +1970,7 @@
   <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1974,11 +1988,11 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2010,99 +2024,99 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -2110,7 +2124,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>35</v>
@@ -2143,7 +2157,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2161,18 +2175,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -2192,101 +2206,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>79</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2316,11 +2328,11 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2358,73 +2370,73 @@
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -2432,13 +2444,13 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2469,11 +2481,11 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2505,79 +2517,79 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -2585,13 +2597,13 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2622,11 +2634,11 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2658,79 +2670,79 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -2738,13 +2750,13 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2757,7 +2769,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H10" sqref="A1:XFD1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2775,18 +2787,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -2806,27 +2818,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2837,16 +2849,16 @@
         <v>29</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="234" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="234" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
@@ -2857,16 +2869,16 @@
         <v>31</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
@@ -2877,30 +2889,28 @@
         <v>34</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="15"/>
+      <c r="C7" s="3">
+        <v>18</v>
+      </c>
       <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="15"/>
+      <c r="G7" s="7">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2912,7 +2922,7 @@
   <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D9" sqref="A1:XFD1048576"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2930,18 +2940,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
@@ -2949,7 +2959,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="3" t="s">
@@ -2962,115 +2972,115 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>132</v>
+      <c r="G7" s="3">
+        <v>9</v>
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>45</v>
+      <c r="C8" s="5">
+        <v>9</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -3084,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H8" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3103,18 +3113,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
@@ -3134,113 +3144,111 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>54</v>
+      <c r="C8" s="5">
+        <v>19</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="H8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3252,7 +3260,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="A1:XFD1048576"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3270,18 +3278,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -3301,101 +3309,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="G4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="90" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="F5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F6" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="15"/>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
       <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="15"/>
+      <c r="G7" s="7">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3406,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC162D1-E2CB-9148-882F-73C6122D3717}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K12" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3421,18 +3427,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -3452,101 +3458,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="162" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="162" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="15"/>
+      <c r="C7" s="3">
+        <v>11</v>
+      </c>
       <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="15"/>
+      <c r="G7" s="7">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3557,8 +3561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87741834-764D-8442-88E6-1252B0C99BC2}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J6" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3574,18 +3578,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -3605,101 +3609,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>134</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3711,7 +3713,7 @@
   <dimension ref="B1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="A1:XFD1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3723,18 +3725,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -3754,74 +3756,73 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>131</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
@@ -3839,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J6" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3854,18 +3855,18 @@
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
@@ -3885,101 +3886,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="162" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="F6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="14" customFormat="1" ht="162" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="14" customFormat="1" ht="108" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>71</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Polished excel for easy comprehention
added correct spacing and adjusted any typo/ error
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627743DF-B64C-1140-9453-AD422756AC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071E6421-A504-2847-AB17-9E727FA21E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="14" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1377,12 +1377,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="15.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="21.83203125" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="15" style="14" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="32.6640625" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -1519,12 +1521,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="17.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="21.6640625" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="21" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="27" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -1670,12 +1674,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="20.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="20.33203125" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
     <col min="6" max="6" width="20" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="28.83203125" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -1821,12 +1827,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="19.83203125" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
     <col min="6" max="6" width="21.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="14.83203125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -2153,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B15306A-7E9E-EF49-BEA7-BC4B3796CCEF}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2795,7 +2803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2948,7 +2956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -3122,7 +3130,7 @@
   <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3130,11 +3138,11 @@
     <col min="1" max="1" width="10.83203125" style="14"/>
     <col min="2" max="2" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="4" max="4" width="20" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
     <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="19.5" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -3295,7 +3303,7 @@
     <col min="1" max="1" width="10.83203125" style="14"/>
     <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="4" max="4" width="15.5" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
     <col min="6" max="6" width="13.1640625" style="14" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
@@ -3445,10 +3453,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="23.33203125" style="15" customWidth="1"/>
     <col min="5" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="25.6640625" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -3594,12 +3604,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="18.1640625" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="14" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="16.5" style="15" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -3745,9 +3757,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
-    <col min="5" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="15.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="17.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="14.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="23.6640625" style="14" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -3873,10 +3891,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="15"/>
-    <col min="5" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="18.83203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="14"/>
+    <col min="6" max="6" width="24.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="21.5" style="15" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
identified and fixed erros within the dataset
bug fixes
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071E6421-A504-2847-AB17-9E727FA21E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10337B5-C53A-6849-8D09-506DA5E732C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" firstSheet="9" activeTab="14" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="193">
   <si>
     <t>Task</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>5min</t>
+  </si>
+  <si>
+    <t>Data Polish (min)</t>
   </si>
 </sst>
 </file>
@@ -1071,15 +1074,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1093,7 +1097,7 @@
         <v>189</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -2161,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B15306A-7E9E-EF49-BEA7-BC4B3796CCEF}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated excel and added Normalisation
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10337B5-C53A-6849-8D09-506DA5E732C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADC47FD-BA41-9D46-94A7-2946DC11DD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1480" windowWidth="27240" windowHeight="14940" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" activeTab="1" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Normalisation" sheetId="2" r:id="rId2"/>
     <sheet name="Missing Values" sheetId="3" r:id="rId3"/>
     <sheet name="Outlier Removal" sheetId="4" r:id="rId4"/>
-    <sheet name="Numeric To Categorical" sheetId="5" r:id="rId5"/>
-    <sheet name="Principal Component Analysis" sheetId="6" r:id="rId6"/>
+    <sheet name="Label encoding" sheetId="5" r:id="rId5"/>
+    <sheet name="binning" sheetId="6" r:id="rId6"/>
     <sheet name="Change Column Type" sheetId="7" r:id="rId7"/>
     <sheet name="Rename Column" sheetId="8" r:id="rId8"/>
     <sheet name="Special Character Removal" sheetId="9" r:id="rId9"/>
@@ -30,9 +30,9 @@
     <sheet name="Tokenization" sheetId="15" r:id="rId15"/>
     <sheet name="Regex (Regular Expressions)" sheetId="16" r:id="rId16"/>
     <sheet name="Datetime Components" sheetId="18" r:id="rId17"/>
-    <sheet name="Remove Columns" sheetId="19" r:id="rId18"/>
+    <sheet name="Remove Duplicates" sheetId="19" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="187">
   <si>
     <t>Task</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Outlier Removal</t>
   </si>
   <si>
-    <t>Numeric to Category</t>
-  </si>
-  <si>
-    <t>Principal Component Analysis</t>
-  </si>
-  <si>
     <t>Change Column Type</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Datetime Components</t>
   </si>
   <si>
-    <t>Remove Columns</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -136,30 +127,15 @@
     <t>df = pd.read_csv('file.csv')</t>
   </si>
   <si>
-    <t>Visualize Data</t>
-  </si>
-  <si>
     <t>10 min</t>
   </si>
   <si>
-    <t>df.describe()</t>
-  </si>
-  <si>
     <t>Apply Normalization</t>
   </si>
   <si>
-    <t>from sklearn.preprocessing import MinMaxScaler &lt;br&gt; scaler = MinMaxScaler() &lt;br&gt; df_scaled = pd.DataFrame(scaler.fit_transform(df), columns=df.columns)</t>
-  </si>
-  <si>
-    <t>Verify Normalization</t>
-  </si>
-  <si>
     <t>2 min</t>
   </si>
   <si>
-    <t>df_scaled.describe()</t>
-  </si>
-  <si>
     <t>Overall</t>
   </si>
   <si>
@@ -211,42 +187,9 @@
     <t>Replot with sns.boxplot(data=df)</t>
   </si>
   <si>
-    <t>Identify Numerics</t>
-  </si>
-  <si>
-    <t>df.select_dtypes(include=['int', 'float'])</t>
-  </si>
-  <si>
-    <t>Convert to Category</t>
-  </si>
-  <si>
-    <t>df['column'] = df['column'].astype('category')</t>
-  </si>
-  <si>
-    <t>df.info() to check new dtypes</t>
-  </si>
-  <si>
-    <t>Standardize Data</t>
-  </si>
-  <si>
     <t>3 min</t>
   </si>
   <si>
-    <t>StandardScaler().fit_transform(df)</t>
-  </si>
-  <si>
-    <t>Apply PCA</t>
-  </si>
-  <si>
-    <t>PCA(n_components=k).fit_transform(scaled_data)</t>
-  </si>
-  <si>
-    <t>Variance Check</t>
-  </si>
-  <si>
-    <t>explained_variance_ratio_ to check variance</t>
-  </si>
-  <si>
     <t>Identify Column &amp; Type</t>
   </si>
   <si>
@@ -394,21 +337,6 @@
     <t>df[['year', 'month', 'day']].head()</t>
   </si>
   <si>
-    <t>Identify Columns</t>
-  </si>
-  <si>
-    <t>df.columns to list all columns</t>
-  </si>
-  <si>
-    <t>Drop Columns</t>
-  </si>
-  <si>
-    <t>df.drop(['column1', 'column2'], axis=1, inplace=True)</t>
-  </si>
-  <si>
-    <t>df.head() to ensure columns are dropped</t>
-  </si>
-  <si>
     <t>Load Data</t>
   </si>
   <si>
@@ -496,36 +424,6 @@
     <t>Re-inspect with 'Data Table' or 'Distributions' widget.</t>
   </si>
   <si>
-    <t>Inspect Numeric Columns</t>
-  </si>
-  <si>
-    <t>Connect 'Data Table' widget to identify numeric columns.</t>
-  </si>
-  <si>
-    <t>Convert Type</t>
-  </si>
-  <si>
-    <t>Use 'Edit Domain' widget to change numeric to categorical.</t>
-  </si>
-  <si>
-    <t>Verify Conversion</t>
-  </si>
-  <si>
-    <t>Re-inspect with 'Data Table' to check the new column type.</t>
-  </si>
-  <si>
-    <t>Use 'Preprocess' widget and select 'Scale'.</t>
-  </si>
-  <si>
-    <t>Connect 'PCA' widget and set parameters.</t>
-  </si>
-  <si>
-    <t>Visualize PCA</t>
-  </si>
-  <si>
-    <t>Connect 'Scatter Plot' widget to the PCA output to visualize components.</t>
-  </si>
-  <si>
     <t>Inspect Text Data</t>
   </si>
   <si>
@@ -610,15 +508,6 @@
     <t>Use 'Date' widget to extract date components.</t>
   </si>
   <si>
-    <t>Inspect Columns</t>
-  </si>
-  <si>
-    <t>Use 'Data Table' to decide which columns to remove.</t>
-  </si>
-  <si>
-    <t>Use 'Select Columns' to deselect unwanted columns.</t>
-  </si>
-  <si>
     <t>Python (min)</t>
   </si>
   <si>
@@ -632,6 +521,99 @@
   </si>
   <si>
     <t>Data Polish (min)</t>
+  </si>
+  <si>
+    <t>Label encoding</t>
+  </si>
+  <si>
+    <t>Remove Duplicates</t>
+  </si>
+  <si>
+    <t>binning</t>
+  </si>
+  <si>
+    <t>Inspect Categorical Data</t>
+  </si>
+  <si>
+    <t>df.select_dtypes(include=['object']).head()</t>
+  </si>
+  <si>
+    <t>Apply Label Encoding</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import LabelEncoder&lt;br&gt;encoder = LabelEncoder()&lt;br&gt;df['encoded_column'] = encoder.fit_transform(df['categorical_column'])</t>
+  </si>
+  <si>
+    <t>df.head()</t>
+  </si>
+  <si>
+    <t>Inspect Numeric Data</t>
+  </si>
+  <si>
+    <t>df['numeric_column'].describe() or df['numeric_column'].plot(kind='hist')</t>
+  </si>
+  <si>
+    <t>Apply Binning</t>
+  </si>
+  <si>
+    <t>bins = [0, 10, 20, 30]&lt;br&gt;labels = ['Low', 'Medium', 'High']&lt;br&gt;df['binned_column'] = pd.cut(df['numeric_column'], bins=bins, labels=labels)</t>
+  </si>
+  <si>
+    <t>df['binned_column'].value_counts()</t>
+  </si>
+  <si>
+    <t>Inspect for Duplicates</t>
+  </si>
+  <si>
+    <t>df.duplicated().sum()</t>
+  </si>
+  <si>
+    <t>df = df.drop_duplicates()</t>
+  </si>
+  <si>
+    <t>df.describe() or df['numeric_column'].hist()</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import MinMaxScaler&lt;br&gt;scaler = MinMaxScaler()&lt;br&gt;df[['numeric_column']] = scaler.fit_transform(df[['numeric_column']])</t>
+  </si>
+  <si>
+    <t>df['numeric_column'].hist()</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' to identify categorical columns.</t>
+  </si>
+  <si>
+    <t>Connect 'Ordinal' widget to convert categories to integers.</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' or 'Histogram' to review distribution of numeric columns.</t>
+  </si>
+  <si>
+    <t>Connect 'Discretize' widget to convert numeric values into bins.</t>
+  </si>
+  <si>
+    <t>Re-inspect with 'Data Table' or 'Histogram'.</t>
+  </si>
+  <si>
+    <t>Use 'Data Table' to look for obvious duplicates.</t>
+  </si>
+  <si>
+    <t>Use 'Remove Duplicates' widget to delete duplicate rows.</t>
+  </si>
+  <si>
+    <t>Upload the dataset to the 'Import' page.</t>
+  </si>
+  <si>
+    <t>Inspect Data</t>
+  </si>
+  <si>
+    <t>Review the data distribution on the 'Data Profiling' page.</t>
+  </si>
+  <si>
+    <t>Apply normalization on the 'Data Cleaning' page.</t>
+  </si>
+  <si>
+    <t>Check the normalized data on the 'Data Profiling' page.</t>
   </si>
 </sst>
 </file>
@@ -727,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -752,6 +734,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1072,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCED56-B1F8-4349-9CA5-CFF48A33C9D8}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1106,7 +1091,7 @@
       </c>
       <c r="B2" s="2">
         <f>Normalisation!C7</f>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <f>Normalisation!G7</f>
@@ -1144,35 +1129,35 @@
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="B5" s="2">
-        <f>'Numeric To Categorical'!C7</f>
-        <v>6</v>
+        <f>'Label encoding'!C7</f>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
-        <f>'Numeric To Categorical'!G7</f>
-        <v>10</v>
+        <f>'Label encoding'!G7</f>
+        <v>8</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="B6" s="2">
-        <f>'Principal Component Analysis'!C7</f>
-        <v>11</v>
+        <f>binning!C7</f>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
-        <f>'Principal Component Analysis'!G7</f>
-        <v>11</v>
+        <f>binning!G7</f>
+        <v>7</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <f>'Change Column Type'!C7</f>
@@ -1186,7 +1171,7 @@
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <f>'Rename Column'!C6</f>
@@ -1200,7 +1185,7 @@
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <f>'Special Character Removal'!C7</f>
@@ -1214,7 +1199,7 @@
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <f>'Trim Whitespace'!C6</f>
@@ -1228,7 +1213,7 @@
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <f>'Replace Substrings'!C7</f>
@@ -1242,7 +1227,7 @@
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <f>'Text Case'!C7</f>
@@ -1256,7 +1241,7 @@
     </row>
     <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <f>'Remove Stopwords'!C7</f>
@@ -1270,7 +1255,7 @@
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <f>'Collapse Rare Categories'!C8</f>
@@ -1284,7 +1269,7 @@
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <f>Tokenization!C7</f>
@@ -1298,7 +1283,7 @@
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <f>'Regex (Regular Expressions)'!C7</f>
@@ -1312,7 +1297,7 @@
     </row>
     <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <f>'Datetime Components'!C8</f>
@@ -1326,45 +1311,51 @@
     </row>
     <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2">
-        <f>'Remove Columns'!C7</f>
-        <v>6</v>
+        <f>'Remove Duplicates'!C7</f>
+        <v>8</v>
       </c>
       <c r="C18" s="2">
-        <f>'Remove Columns'!G7</f>
+        <f>'Remove Duplicates'!G7</f>
         <v>8</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <f>SUM(B2:B18)</f>
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1">
         <f>B19/60</f>
-        <v>2.6333333333333333</v>
+        <v>2.4833333333333334</v>
       </c>
       <c r="C20" s="1">
         <f>C19/60</f>
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1381,24 +1372,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="15.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="21.83203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="32.6640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -1407,104 +1393,104 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="144" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>8</v>
@@ -1525,24 +1511,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="17.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="21.6640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="17.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="27" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -1551,113 +1532,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="144" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>9</v>
@@ -1678,24 +1659,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="20.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="20.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="20" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="28.83203125" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -1704,113 +1680,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>7</v>
@@ -1826,29 +1802,29 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="19.83203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="21.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="23.6640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="18.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="15"/>
+    <col min="4" max="4" width="19.83203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="15"/>
+    <col min="6" max="6" width="21.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="23.6640625" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -1857,113 +1833,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="90" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>8</v>
@@ -1984,24 +1960,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="19.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="18.83203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="17.5" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2010,133 +1981,133 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3">
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3">
         <v>13</v>
@@ -2171,24 +2142,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="14.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="20.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="20.1640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2197,113 +2163,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>8</v>
@@ -2324,24 +2290,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="19.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="20" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="20" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="14" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2350,113 +2311,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>8</v>
@@ -2477,24 +2438,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="24.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="24" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="24.1640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2503,116 +2459,116 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>190</v>
+        <v>44</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>7</v>
@@ -2620,7 +2576,7 @@
     </row>
     <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3">
         <v>12</v>
@@ -2652,147 +2608,146 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836C7B9-0B85-3A4B-822E-23EEAE7381E3}">
-  <dimension ref="B1:K7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="24.5" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="24.5" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="14" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="54" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>8</v>
@@ -2805,150 +2760,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE17A0E3-F5EC-554A-9735-BFFAD7E9361A}">
-  <dimension ref="B1:K7"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="15.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="25" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="22.6640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="15"/>
+    <col min="4" max="4" width="15.1640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="15"/>
+    <col min="6" max="6" width="25" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="22.6640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="15"/>
+    <col min="10" max="10" width="14.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="2:12" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="90" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
+      <c r="J3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="198" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="108" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="234" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="54" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C7" s="3">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7">
         <v>8</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2960,30 +2971,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C172AB-F034-AC4C-971B-243D9D7B901D}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="19.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="41.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="25" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="21.5" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -2992,86 +2999,86 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="4" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
@@ -3079,44 +3086,44 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>9</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5">
         <v>9</v>
@@ -3139,24 +3146,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="20" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="19.5" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="14" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -3165,116 +3167,116 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>13</v>
@@ -3282,7 +3284,7 @@
     </row>
     <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5">
         <v>19</v>
@@ -3304,24 +3306,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="15.5" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="13.1640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="16.33203125" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="19" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="15"/>
+    <col min="4" max="4" width="15.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="15"/>
+    <col min="6" max="6" width="20" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="16.33203125" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -3330,116 +3332,116 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="90" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="198" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>55</v>
+        <v>162</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3451,28 +3453,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC162D1-E2CB-9148-882F-73C6122D3717}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="23.33203125" style="15" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="25.6640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="16" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="15"/>
+    <col min="6" max="6" width="19.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -3481,116 +3485,116 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="90" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>164</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>57</v>
+        <v>164</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="144" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="162" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>63</v>
+        <v>168</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3608,24 +3612,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="18.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="20.83203125" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -3634,113 +3633,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>8</v>
@@ -3761,24 +3760,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="15.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="17.6640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="14.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="23.6640625" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -3787,98 +3781,98 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="90" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3895,24 +3889,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="18.83203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="24.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="21.5" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D1" s="10"/>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10"/>
       <c r="K1" s="9" t="s">
@@ -3921,113 +3910,113 @@
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="162" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>10</v>

</xml_diff>

<commit_message>
added change column type
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D206EB-970B-4E4D-B459-E7209E316288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DFB208-FF76-5641-BF62-382C3CEA2947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" activeTab="3" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" activeTab="6" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="206">
   <si>
     <t>Task</t>
   </si>
@@ -662,6 +662,15 @@
   </si>
   <si>
     <t>Validate removal on the 'Data Profiling' page.</t>
+  </si>
+  <si>
+    <t>Review column types on the 'Data Profiling' page.</t>
+  </si>
+  <si>
+    <t>Change column types on the 'Data Cleaning' page.</t>
+  </si>
+  <si>
+    <t>Confirm type changes on the 'Data Profiling' page.</t>
   </si>
 </sst>
 </file>
@@ -3298,7 +3307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6030CA5-24BA-8741-A5E3-0CBEB6E20D49}">
   <dimension ref="B1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
@@ -3929,10 +3938,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87741834-764D-8442-88E6-1252B0C99BC2}">
-  <dimension ref="B1:K7"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3943,7 +3952,7 @@
     <col min="8" max="8" width="20.83203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>101</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
@@ -3975,8 +3984,17 @@
       <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
@@ -3995,8 +4013,17 @@
       <c r="H3" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="J3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
@@ -4015,8 +4042,17 @@
       <c r="H4" s="8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="J4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>47</v>
       </c>
@@ -4035,8 +4071,17 @@
       <c r="H5" s="8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="90" x14ac:dyDescent="0.2">
+      <c r="J5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
@@ -4055,8 +4100,17 @@
       <c r="H6" s="8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="J6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
@@ -4069,6 +4123,13 @@
       <c r="G7" s="3">
         <v>8</v>
       </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="3">
+        <v>4</v>
+      </c>
+      <c r="L7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added special character results
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2A619A-55EF-A24B-B5AE-C278D3459160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456BAAF8-20EE-6A45-844E-BD0F5CC210B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" activeTab="7" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" activeTab="8" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="212">
   <si>
     <t>Task</t>
   </si>
@@ -680,6 +680,15 @@
   </si>
   <si>
     <t>Check new names on the 'Data Profiling' page.</t>
+  </si>
+  <si>
+    <t>Spot special characters on the 'Data Profiling' page.</t>
+  </si>
+  <si>
+    <t>Remove special characters on the 'Data Cleaning' page.</t>
+  </si>
+  <si>
+    <t>Inspect cleaned data on the 'Data Profiling' page.</t>
   </si>
 </sst>
 </file>
@@ -4151,7 +4160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC10668-04B2-D949-B9DB-65DF0C8FBDE5}">
   <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -4335,10 +4344,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8945ED-BAF2-C34A-80C4-D30B68C8DA2C}">
-  <dimension ref="B1:K7"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4347,9 +4356,11 @@
     <col min="4" max="4" width="18.83203125" style="14" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.5" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>101</v>
       </c>
@@ -4361,8 +4372,9 @@
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="2:12" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
@@ -4381,8 +4393,17 @@
       <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
@@ -4401,8 +4422,17 @@
       <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="J3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>53</v>
       </c>
@@ -4421,8 +4451,17 @@
       <c r="H4" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="162" x14ac:dyDescent="0.2">
+      <c r="J4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>55</v>
       </c>
@@ -4441,8 +4480,17 @@
       <c r="H5" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="J5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
@@ -4461,8 +4509,17 @@
       <c r="H6" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="J6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
@@ -4475,6 +4532,13 @@
       <c r="G7" s="3">
         <v>10</v>
       </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added collapse rare category
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS-Polish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB221AF7-9931-B54D-A0EB-21BCCB1F4A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FFD15B-33B6-6A43-86B5-D20C07735CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" firstSheet="4" activeTab="12" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="14940" firstSheet="6" activeTab="13" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="226">
   <si>
     <t>Task</t>
   </si>
@@ -722,6 +722,15 @@
   </si>
   <si>
     <t>Remove stopwords on the 'Data Cleaning' page.</t>
+  </si>
+  <si>
+    <t>Examine category frequencies on the 'Data Profiling' page.</t>
+  </si>
+  <si>
+    <t>Collapse rare categories on the 'Data Cleaning' page.</t>
+  </si>
+  <si>
+    <t>Check collapsed categories on the 'Data Profiling' page.</t>
   </si>
 </sst>
 </file>
@@ -2084,7 +2093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18058F80-552A-2B46-9A61-17D28D671D7E}">
   <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -2289,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990E6A3-2F89-4543-9085-4F79AE6CF6C1}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2301,9 +2310,11 @@
     <col min="4" max="4" width="18.83203125" style="14" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>101</v>
       </c>
@@ -2315,8 +2326,9 @@
       <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="2:12" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
@@ -2335,8 +2347,17 @@
       <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="54" x14ac:dyDescent="0.2">
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
@@ -2355,8 +2376,17 @@
       <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.2">
+      <c r="J3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>73</v>
       </c>
@@ -2375,8 +2405,17 @@
       <c r="H4" s="8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="72" x14ac:dyDescent="0.2">
+      <c r="J4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -2395,8 +2434,17 @@
       <c r="H5" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="J5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="108" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>77</v>
       </c>
@@ -2415,8 +2463,17 @@
       <c r="H6" s="8" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="J6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>42</v>
       </c>
@@ -2435,8 +2492,15 @@
       <c r="H7" s="8" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="3">
+        <v>6</v>
+      </c>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
@@ -2450,17 +2514,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>

</xml_diff>